<commit_message>
SoE tables for all outcomes
1) Analysis.R include code to create a data frame with summary data for all outcomes, comparisons and evaluations for SoE
2) Markdown to incorporate these changes.
To do: refinements needed and correct any potential mistakes
</commit_message>
<xml_diff>
--- a/data/rob_secondary_2024.01.23.xlsx
+++ b/data/rob_secondary_2024.01.23.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sksiafis/Documents/GitHub/LSR3_taar1_H/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0AF72B-10DC-C840-8826-22BEEADF8BB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E782872-DB5D-E449-A330-36D8A380F00C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="500" windowWidth="22220" windowHeight="15700" xr2:uid="{5B321493-8628-1E4C-935B-6CFC743B201E}"/>
+    <workbookView xWindow="21260" yWindow="-21100" windowWidth="22220" windowHeight="15700" xr2:uid="{5B321493-8628-1E4C-935B-6CFC743B201E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="9" r:id="rId1"/>
@@ -659,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{572FBEC7-01CF-B040-AE68-30BAA13155EF}">
   <dimension ref="A1:J88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>